<commit_message>
Update status of block not moved during shimming D
</commit_message>
<xml_diff>
--- a/model-03/shimming_list/2023-08-08_delta_sabia_shimmingD_21periods.xlsx
+++ b/model-03/shimming_list/2023-08-08_delta_sabia_shimmingD_21periods.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas.francisco\data\2023-08-1-DeltaSabia-ShimD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas.francisco\data\lnls-ima\id-sabia\model-03\shimming_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DBBF522-ABE2-49DC-B3E6-056688EA5500}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC3B4229-63FB-441D-B312-744C201C7689}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CIE" sheetId="2" r:id="rId1"/>
@@ -1955,7 +1955,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:T102"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7161,7 +7161,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T102"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A84" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="Q94" sqref="Q94"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -11952,11 +11954,11 @@
         <v>0.25</v>
       </c>
       <c r="P94" s="24">
-        <v>4.9999999999999989E-2</v>
+        <v>0</v>
       </c>
       <c r="Q94" s="24">
         <f t="shared" si="8"/>
-        <v>0.3</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="95" spans="1:17" x14ac:dyDescent="0.25">
@@ -12146,7 +12148,7 @@
       </c>
       <c r="N98" s="11"/>
       <c r="O98" s="14">
-        <f t="shared" ref="O98:O129" si="9">M98+N98</f>
+        <f t="shared" ref="O98:O102" si="9">M98+N98</f>
         <v>0.25</v>
       </c>
       <c r="P98" s="11"/>

</xml_diff>